<commit_message>
Corrections as per comments from mentor
</commit_message>
<xml_diff>
--- a/ДЗ2_Крупа.xlsx
+++ b/ДЗ2_Крупа.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
-    <sheet name="НФ1" sheetId="1" r:id="rId1"/>
+    <sheet name="ДЗ2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>Хрещатик 1</t>
   </si>
@@ -77,19 +77,37 @@
     <t>2НФ</t>
   </si>
   <si>
-    <t>Customes</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
     <t>Products</t>
   </si>
   <si>
     <t>3НФ</t>
   </si>
   <si>
-    <t>Customers</t>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>client_id</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Order_Item</t>
   </si>
 </sst>
 </file>
@@ -99,17 +117,9 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -149,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,11 +191,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -196,16 +232,28 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -235,8 +283,8 @@
       <xdr:rowOff>119743</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>581537</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>268573</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>105791</xdr:rowOff>
     </xdr:to>
@@ -268,19 +316,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>557893</xdr:colOff>
+      <xdr:colOff>1091046</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>173181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>890607</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>104167</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>658916</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>163157</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPr id="7" name="Рисунок 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -293,37 +341,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="557893" y="6014357"/>
-          <a:ext cx="5285714" cy="4866667"/>
+          <a:off x="1091046" y="6199908"/>
+          <a:ext cx="7257143" cy="3990476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>122465</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>2181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>282678</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>102989</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>779318</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>11392</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPr id="9" name="Рисунок 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -336,46 +379,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7021285" y="6136822"/>
-          <a:ext cx="2800000" cy="3409524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>97971</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>333019</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>14667</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7024007" y="9525000"/>
-          <a:ext cx="2847619" cy="2409524"/>
+          <a:off x="9611591" y="6219408"/>
+          <a:ext cx="3151909" cy="7248211"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -650,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,19 +671,23 @@
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -697,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -781,29 +790,29 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="F12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -823,7 +832,7 @@
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>13</v>
@@ -901,7 +910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>103</v>
       </c>
@@ -919,163 +928,207 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="20" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="D21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="I21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="E21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="6" t="s">
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22"/>
+      <c r="D22" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G22"/>
-      <c r="H22" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="G22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22"/>
       <c r="I22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>101</v>
+      <c r="K22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="2">
-        <v>3</v>
-      </c>
-      <c r="D23"/>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
       <c r="E23" s="2">
         <v>101</v>
       </c>
       <c r="F23" s="3">
         <v>45000</v>
       </c>
-      <c r="G23"/>
-      <c r="H23" s="2">
-        <v>101</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>101</v>
+      <c r="K23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
+      <c r="N23" s="4">
+        <v>1</v>
+      </c>
+      <c r="O23" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="2">
-        <v>2</v>
-      </c>
-      <c r="D24"/>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
       <c r="E24" s="2">
         <v>102</v>
       </c>
       <c r="F24" s="3">
         <v>45001</v>
       </c>
-      <c r="G24"/>
-      <c r="H24" s="2">
-        <v>102</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>1</v>
+      <c r="G24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24" s="2">
+        <v>2</v>
       </c>
       <c r="J24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K24"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>102</v>
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
+      <c r="N24" s="4">
+        <v>2</v>
+      </c>
+      <c r="O24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25"/>
+      <c r="D25" s="4">
+        <v>3</v>
+      </c>
       <c r="E25" s="2">
         <v>103</v>
       </c>
       <c r="F25" s="3">
         <v>45002</v>
       </c>
-      <c r="G25"/>
-      <c r="H25" s="2">
-        <v>103</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>2</v>
+      <c r="G25" s="2">
+        <v>3</v>
+      </c>
+      <c r="H25"/>
+      <c r="I25" s="2">
+        <v>3</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K25"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>103</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="2">
-        <v>4</v>
-      </c>
+      <c r="M25" s="4">
+        <v>2</v>
+      </c>
+      <c r="N25" s="4">
+        <v>3</v>
+      </c>
+      <c r="O25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
@@ -1084,8 +1137,17 @@
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26" s="4">
+        <v>3</v>
+      </c>
+      <c r="N26" s="4">
+        <v>2</v>
+      </c>
+      <c r="O26" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -1098,9 +1160,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
@@ -1113,14 +1173,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:G21"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A20:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>